<commit_message>
Tidy sheets a little as per new code structure
Don't need to repeat data between sheets, which I had been doing in the
interim phase.
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_default.xlsx
+++ b/autumn/xls/programs_default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="country_constants" sheetId="1" r:id="rId1"/>
@@ -2258,8 +2258,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2290,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="34">
-        <v>6.7</v>
+        <v>15</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>38</v>
@@ -2367,7 +2367,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="35">
-        <v>0.22</v>
+        <v>0.4</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>46</v>
@@ -2411,7 +2411,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="46">
-        <v>190000</v>
+        <v>1000000</v>
       </c>
       <c r="C13" s="45" t="s">
         <v>62</v>
@@ -2441,7 +2441,7 @@
   </sheetPr>
   <dimension ref="A1:BN38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Move default sheets to same file
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_default.xlsx
+++ b/autumn/xls/programs_default.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807"/>
   </bookViews>
   <sheets>
-    <sheet name="time_variants" sheetId="2" r:id="rId1"/>
-    <sheet name="dropdown_lists" sheetId="3" r:id="rId2"/>
+    <sheet name="default_constants" sheetId="4" r:id="rId1"/>
+    <sheet name="time_variants" sheetId="2" r:id="rId2"/>
+    <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
   <si>
     <t>program_prop_lowquality</t>
   </si>
@@ -168,16 +169,248 @@
   </si>
   <si>
     <t>scenario_9</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>tb_n_contact</t>
+  </si>
+  <si>
+    <t>Effective contact rate for TB</t>
+  </si>
+  <si>
+    <t>tb_multiplier_force_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearpos</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated</t>
+  </si>
+  <si>
+    <t>tb_prop_amplification</t>
+  </si>
+  <si>
+    <t>tb_multiplier_latency_protection</t>
+  </si>
+  <si>
+    <t>Relative risk of infection in those already latently infected</t>
+  </si>
+  <si>
+    <t>tb_multiplier_bcg_protection</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_early_latent</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_activeuntreated</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_rate_late_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_ipt_effectiveness</t>
+  </si>
+  <si>
+    <t>Relative risk of TB in those treated with IPT (i.e. lower value more effective)</t>
+  </si>
+  <si>
+    <t>tb_prop_ltbi_test_sensitivity</t>
+  </si>
+  <si>
+    <t>tb_prop_contacts_infected</t>
+  </si>
+  <si>
+    <t>program_timeperiod_await_treatment_smearneg_xpert</t>
+  </si>
+  <si>
+    <t>program_rate_start_treatment</t>
+  </si>
+  <si>
+    <t>Inverse of time period that detected patients have to wait before starting treatment</t>
+  </si>
+  <si>
+    <t>program_rate_restart_presenting</t>
+  </si>
+  <si>
+    <t>Rate at which patients who were told they didn't have TB turn up again to the health system</t>
+  </si>
+  <si>
+    <t>program_rate_leavelowquality</t>
+  </si>
+  <si>
+    <t>Rate at which patients change from the low quality to the high quality health system</t>
+  </si>
+  <si>
+    <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>Proportion of TB-related deaths not already under treatment that are correctly reported as such</t>
+  </si>
+  <si>
+    <t>demo_household_size</t>
+  </si>
+  <si>
+    <t>*this is Fiji's household size in 2008</t>
+  </si>
+  <si>
+    <t>time_step</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>Calendar year from which model starts running (i.e. when TB is introduced)</t>
+  </si>
+  <si>
+    <t>scenario_start_time</t>
+  </si>
+  <si>
+    <t>Time that scenarios start to be implemented (probably make these modifiable for each program later)</t>
+  </si>
+  <si>
+    <t>scenario_full_time</t>
+  </si>
+  <si>
+    <t>Time that scenarios reach full effect</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB first begins to emerge</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB amplification reaches full parameter value</t>
+  </si>
+  <si>
+    <t>timepoint_introduce_xdr</t>
+  </si>
+  <si>
+    <t>Calendar year that XDR-TB first emerged</t>
+  </si>
+  <si>
+    <t>recent_time</t>
+  </si>
+  <si>
+    <t>current_time</t>
+  </si>
+  <si>
+    <t>scenario_end_time</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>Starting population of fully susceptible persons (essentially the starting population size)</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Seed of patients with active TB</t>
+  </si>
+  <si>
+    <t>n_organs</t>
+  </si>
+  <si>
+    <t>n_strains</t>
+  </si>
+  <si>
+    <t>n_comorbidities</t>
+  </si>
+  <si>
+    <t>is_lowquality</t>
+  </si>
+  <si>
+    <t>is_amplification</t>
+  </si>
+  <si>
+    <t>is_misassignment</t>
+  </si>
+  <si>
+    <t>is_additional_diagnostics</t>
+  </si>
+  <si>
+    <t>fitting_method</t>
+  </si>
+  <si>
+    <t>default_smoothness</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>runge_kutta</t>
+  </si>
+  <si>
+    <t>scenarios_to_run</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Don't change this - change through control panel please</t>
+  </si>
+  <si>
+    <t>age_breakpoints</t>
+  </si>
+  <si>
+    <t>scipy</t>
+  </si>
+  <si>
+    <t>explicit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +494,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,8 +615,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -424,8 +703,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1089,8 +1403,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1131,10 +1446,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="11" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 2 2" xfId="5"/>
+    <cellStyle name="Input" xfId="663" builtinId="20"/>
     <cellStyle name="Input 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="6"/>
@@ -2094,12 +2447,617 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="39">
+        <v>15</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="39">
+        <v>0.24</v>
+      </c>
+      <c r="C3" s="40"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="39">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="C4" s="40"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="39">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="40"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="40"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="40"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="39">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C8" s="40"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="39">
+        <v>0.21</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="40"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="39">
+        <f>60/365.251</f>
+        <v>0.16427059747954148</v>
+      </c>
+      <c r="C11" s="40"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="39">
+        <v>3</v>
+      </c>
+      <c r="C12" s="40"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="40"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="39">
+        <v>2</v>
+      </c>
+      <c r="C14" s="40"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="39">
+        <v>3</v>
+      </c>
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="39">
+        <v>3</v>
+      </c>
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="39">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C17" s="40"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="39">
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="39">
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C19" s="40"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="39">
+        <v>2</v>
+      </c>
+      <c r="C20" s="40"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="39">
+        <f>6.8/1000000*365</f>
+        <v>2.4819999999999998E-3</v>
+      </c>
+      <c r="C21" s="40"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="41">
+        <v>0.4</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="40"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="41">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="C24" s="40"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="41">
+        <f>1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C25" s="40"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="39">
+        <v>26</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="39">
+        <v>4</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="39">
+        <v>2</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="45">
+        <v>4.7</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="46">
+        <v>0.01</v>
+      </c>
+      <c r="C31" s="46"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="48">
+        <v>1895</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="48">
+        <v>2016</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="48">
+        <v>2020</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="50">
+        <v>1945</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="50">
+        <v>1955</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="50">
+        <v>2050</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="48">
+        <v>1990</v>
+      </c>
+      <c r="C38" s="47"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="48">
+        <v>2015</v>
+      </c>
+      <c r="C39" s="47"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="48">
+        <v>2016</v>
+      </c>
+      <c r="C40" s="47"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="48">
+        <v>2020</v>
+      </c>
+      <c r="C41" s="47"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="48">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="47"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="52">
+        <v>1000000</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="54">
+        <v>3</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="56">
+        <v>3</v>
+      </c>
+      <c r="C45" s="55"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="56">
+        <v>0</v>
+      </c>
+      <c r="C46" s="55"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="58">
+        <v>0</v>
+      </c>
+      <c r="C47" s="57"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="55"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="55"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="C50" s="55"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="C51" s="57"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="60">
+        <v>5</v>
+      </c>
+      <c r="C52" s="61"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="62">
+        <v>1</v>
+      </c>
+      <c r="C53" s="61"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="61"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32:B42">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B47 B52">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$D$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B55</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B48:B51</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:BN38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3645,32 +4603,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renaming tabs for consistency
</commit_message>
<xml_diff>
--- a/autumn/xls/programs_default.xlsx
+++ b/autumn/xls/programs_default.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807"/>
   </bookViews>
   <sheets>
-    <sheet name="default_constants" sheetId="4" r:id="rId1"/>
+    <sheet name="constants" sheetId="4" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,7 +4611,7 @@
   <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>